<commit_message>
avanzando clases y relaciones
</commit_message>
<xml_diff>
--- a/Herencias y relaciones.xlsx
+++ b/Herencias y relaciones.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="relaciones" sheetId="1" r:id="rId1"/>
+    <sheet name="pruebas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -265,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0">
+    <comment ref="A20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -289,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -310,6 +311,332 @@
           </rPr>
           <t xml:space="preserve">
 registrara un historico de cada operacion</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Adelson</author>
+  </authors>
+  <commentList>
+    <comment ref="K2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se genera al crear el prestamo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sera para cuando se castigue el cliente, se descuente el interes pendiente.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se genera al crear el prestamo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se genera al momento de crear el prestamo y se va recarculando por cada pago.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se genera al crear el prestamo y se va recalculando por cada movimiento</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Adelson:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">se genera al momento de crear el prestamo y se va recarculando por cada pago.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+en el caso que se cancele un recibo, se captura la cuotaid y el interes, capital y demas y se aplica con signo negativo en cada campo correspondiente. 
+Los recibos se actualizan de este detalle.
+Las cuotas se actualizan de este detalle.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se va generando cada dia, siempre que este vencida la cuota.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+para cuando se castigue un cliente o prestamo descontar el interes por aqui. Al castigar se especificara una cuota de inicio del descuento y se captura la cuotaid, la mora y el interes y se aplica como un descuento.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Se genero la mora del dia 6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se genero la mora del dia 7</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Adelson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+se creo un recibo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Adelson:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>modo de cancelar un recibo. De este modo puedes cancelar cualquier recibo, sin importar el orden.</t>
         </r>
       </text>
     </comment>
@@ -318,7 +645,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>id</t>
   </si>
@@ -453,13 +780,76 @@
   </si>
   <si>
     <t>Cerveseria</t>
+  </si>
+  <si>
+    <t>fechapago</t>
+  </si>
+  <si>
+    <t>cuotano</t>
+  </si>
+  <si>
+    <t>morag</t>
+  </si>
+  <si>
+    <t>morar</t>
+  </si>
+  <si>
+    <t>morad</t>
+  </si>
+  <si>
+    <t>moraxc</t>
+  </si>
+  <si>
+    <t>interesg</t>
+  </si>
+  <si>
+    <t>interesr</t>
+  </si>
+  <si>
+    <t>interesxc</t>
+  </si>
+  <si>
+    <t>capitalg</t>
+  </si>
+  <si>
+    <t>capitalr</t>
+  </si>
+  <si>
+    <t>capitalxc</t>
+  </si>
+  <si>
+    <t>totalg</t>
+  </si>
+  <si>
+    <t>totalr</t>
+  </si>
+  <si>
+    <t>totalxc</t>
+  </si>
+  <si>
+    <t>interesd</t>
+  </si>
+  <si>
+    <t>totald</t>
+  </si>
+  <si>
+    <t>cuotaID</t>
+  </si>
+  <si>
+    <t>montocuota</t>
+  </si>
+  <si>
+    <t>Generado</t>
+  </si>
+  <si>
+    <t>reciboID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +886,33 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -523,7 +940,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -531,11 +948,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -578,6 +1004,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,7 +1294,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -858,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,12 +1322,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
@@ -924,12 +1368,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -1021,178 +1465,173 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15"/>
-    </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>13</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>31</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>32</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H20" t="s">
         <v>33</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I20" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-    </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="19"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
     </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
     <row r="28" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
+      <c r="A28" s="1"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E30" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G30" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="3">
-        <v>1</v>
-      </c>
-      <c r="D30" s="10">
-        <v>43427</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="3">
-        <v>2</v>
-      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>16</v>
@@ -1204,24 +1643,332 @@
         <v>43427</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G31" s="3">
         <v>2</v>
       </c>
     </row>
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>2</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10">
+        <v>43427</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>20</v>
+      </c>
+      <c r="B3" s="21">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21">
+        <v>5</v>
+      </c>
+      <c r="F3" s="21">
+        <v>200</v>
+      </c>
+      <c r="K3" s="21">
+        <v>50</v>
+      </c>
+      <c r="O3" s="21">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>21</v>
+      </c>
+      <c r="B4" s="21">
+        <v>2</v>
+      </c>
+      <c r="C4" s="21">
+        <v>10</v>
+      </c>
+      <c r="F4" s="21">
+        <v>150</v>
+      </c>
+      <c r="K4" s="21">
+        <v>25</v>
+      </c>
+      <c r="O4" s="21">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>1</v>
+      </c>
+      <c r="B11" s="21">
+        <v>20</v>
+      </c>
+      <c r="C11" s="21">
+        <v>6</v>
+      </c>
+      <c r="D11" s="21">
+        <v>5</v>
+      </c>
+      <c r="J11" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <v>2</v>
+      </c>
+      <c r="B12" s="21">
+        <v>20</v>
+      </c>
+      <c r="C12" s="21">
+        <v>7</v>
+      </c>
+      <c r="D12" s="21">
+        <v>10</v>
+      </c>
+      <c r="J12" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>3</v>
+      </c>
+      <c r="B13" s="21">
+        <v>20</v>
+      </c>
+      <c r="C13" s="21">
+        <v>7</v>
+      </c>
+      <c r="E13" s="23">
+        <v>10</v>
+      </c>
+      <c r="F13" s="21">
+        <v>5</v>
+      </c>
+      <c r="G13" s="21">
+        <v>50</v>
+      </c>
+      <c r="I13" s="21">
+        <v>50</v>
+      </c>
+      <c r="J13" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <v>4</v>
+      </c>
+      <c r="B14" s="21">
+        <v>20</v>
+      </c>
+      <c r="C14" s="21">
+        <v>10</v>
+      </c>
+      <c r="E14" s="21">
+        <v>-10</v>
+      </c>
+      <c r="F14" s="21">
+        <v>-5</v>
+      </c>
+      <c r="G14" s="21">
+        <v>-50</v>
+      </c>
+      <c r="I14" s="21">
+        <v>-50</v>
+      </c>
+      <c r="J14" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
normalizando base de datos
</commit_message>
<xml_diff>
--- a/Herencias y relaciones.xlsx
+++ b/Herencias y relaciones.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="relaciones" sheetId="1" r:id="rId1"/>
     <sheet name="pruebas" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -645,7 +646,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="134">
   <si>
     <t>id</t>
   </si>
@@ -843,6 +844,210 @@
   </si>
   <si>
     <t>reciboID</t>
+  </si>
+  <si>
+    <t>residencia</t>
+  </si>
+  <si>
+    <t>cedula</t>
+  </si>
+  <si>
+    <t>pasaporte</t>
+  </si>
+  <si>
+    <t>estado_civil</t>
+  </si>
+  <si>
+    <t>nacimiento</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>ocupacion</t>
+  </si>
+  <si>
+    <t>nacionalidad</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direccion </t>
+  </si>
+  <si>
+    <t>dependiente</t>
+  </si>
+  <si>
+    <t>otros</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>telefono1</t>
+  </si>
+  <si>
+    <t>telefono2</t>
+  </si>
+  <si>
+    <t>correo1</t>
+  </si>
+  <si>
+    <t>correo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adelson </t>
+  </si>
+  <si>
+    <t>arquilada</t>
+  </si>
+  <si>
+    <t>union libre</t>
+  </si>
+  <si>
+    <t>hombre</t>
+  </si>
+  <si>
+    <t>dominicana</t>
+  </si>
+  <si>
+    <t>herrera</t>
+  </si>
+  <si>
+    <t>calle jose reyes no. 35 el palmar de herrera</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>adelsanchez67@yahoo.es</t>
+  </si>
+  <si>
+    <t>concentra cid</t>
+  </si>
+  <si>
+    <t>credifacil</t>
+  </si>
+  <si>
+    <t>rosalis</t>
+  </si>
+  <si>
+    <t>felix</t>
+  </si>
+  <si>
+    <t>rosa</t>
+  </si>
+  <si>
+    <t>referencia2</t>
+  </si>
+  <si>
+    <t>mujer</t>
+  </si>
+  <si>
+    <t>cajera</t>
+  </si>
+  <si>
+    <t>repuesto los pena</t>
+  </si>
+  <si>
+    <t>adelson</t>
+  </si>
+  <si>
+    <t>conyuge_celular</t>
+  </si>
+  <si>
+    <t>garante_celular</t>
+  </si>
+  <si>
+    <t>yudy</t>
+  </si>
+  <si>
+    <t>usuario_clave</t>
+  </si>
+  <si>
+    <t>empresa_telefono</t>
+  </si>
+  <si>
+    <t>empresa_telefono2</t>
+  </si>
+  <si>
+    <t>empleador_telefono</t>
+  </si>
+  <si>
+    <t>clienteID</t>
+  </si>
+  <si>
+    <t>celular</t>
+  </si>
+  <si>
+    <t>telefonos</t>
+  </si>
+  <si>
+    <t>correos</t>
+  </si>
+  <si>
+    <t>casada</t>
+  </si>
+  <si>
+    <t>referenciaID</t>
+  </si>
+  <si>
+    <t>empresaID</t>
+  </si>
+  <si>
+    <t>adel8021@gmail.com</t>
+  </si>
+  <si>
+    <t>referencia</t>
+  </si>
+  <si>
+    <t>haitiano</t>
+  </si>
+  <si>
+    <t>el coco</t>
+  </si>
+  <si>
+    <t>rosalis@unicaribe.edu.do</t>
+  </si>
+  <si>
+    <t>desarrollador</t>
+  </si>
+  <si>
+    <t>el palmar</t>
+  </si>
+  <si>
+    <t>persona</t>
+  </si>
+  <si>
+    <t>usuarioID</t>
+  </si>
+  <si>
+    <t>empleadorID</t>
+  </si>
+  <si>
+    <t>conyugeID</t>
+  </si>
+  <si>
+    <t>garanteID</t>
+  </si>
+  <si>
+    <t>referencia1</t>
+  </si>
+  <si>
+    <t>referencia_Telefono</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>domingo</t>
+  </si>
+  <si>
+    <t>5522666998</t>
+  </si>
+  <si>
+    <t>4452588555</t>
   </si>
 </sst>
 </file>
@@ -961,7 +1166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1004,9 +1209,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1022,6 +1224,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,7 +1513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1304,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1322,12 +1541,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
@@ -1368,12 +1587,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -1475,11 +1694,11 @@
       <c r="A17"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -1569,7 +1788,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="18"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
@@ -1691,278 +1910,278 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+      <c r="A3" s="20">
         <v>20</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="20">
         <v>1</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>5</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <v>200</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="20">
         <v>50</v>
       </c>
-      <c r="O3" s="21">
+      <c r="O3" s="20">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>21</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="20">
         <v>2</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>10</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <v>150</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="20">
         <v>25</v>
       </c>
-      <c r="O4" s="21">
+      <c r="O4" s="20">
         <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="21"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>1</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>20</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>6</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="20">
         <v>5</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>2</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>20</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>7</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>10</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="20">
         <v>3</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>20</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>7</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <v>10</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>5</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="20">
         <v>50</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <v>50</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>4</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>20</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>10</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>-10</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>-5</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="20">
         <v>-50</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="20">
         <v>-50</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="20">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="20">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="20">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="20">
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="20">
         <v>11</v>
       </c>
     </row>
@@ -1971,4 +2190,750 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z1" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB1" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF1" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG1" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="18">
+        <v>1201103502</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="26">
+        <v>33095</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="18">
+        <v>2</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="P2" s="18">
+        <v>64545445</v>
+      </c>
+      <c r="Q2" s="18">
+        <v>64545666</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="T2" t="s">
+        <v>116</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="V2" s="18">
+        <v>8298852224</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="18">
+        <v>854</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA2" s="18">
+        <v>55866224589</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="18">
+        <v>8298922597</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="18">
+        <v>5452584566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="18">
+        <v>21545656</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="26">
+        <v>32194</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="18">
+        <v>2</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="18">
+        <v>54545454</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>54545877</v>
+      </c>
+      <c r="R3" s="18">
+        <v>8496364367</v>
+      </c>
+      <c r="S3" t="s">
+        <v>120</v>
+      </c>
+      <c r="U3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="18">
+        <v>8298852224</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" s="18">
+        <v>854</v>
+      </c>
+      <c r="Z3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA3" s="18">
+        <v>55866656558</v>
+      </c>
+      <c r="AB3" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC3" s="18">
+        <v>8496364367</v>
+      </c>
+      <c r="AD3" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE3" s="18">
+        <v>54225585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>1</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1201103502</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="28">
+        <v>33095</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" s="27">
+        <v>2</v>
+      </c>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="P7" s="18"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27">
+        <v>21545656</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="28">
+        <v>32194</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="27">
+        <v>2</v>
+      </c>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="P8" s="18"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="18">
+        <v>854</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="18">
+        <v>64545445</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="18">
+        <v>64545666</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="18">
+        <v>54545454</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="18">
+        <v>54545877</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="18">
+        <v>55866224589</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="18">
+        <v>8298852224</v>
+      </c>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="18">
+        <v>55866656558</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F23" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="T24" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="U24" s="18">
+        <v>54225585</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="18">
+        <v>8298922597</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="L25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="18">
+        <v>8298922597</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="18">
+        <v>8496364367</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="18">
+        <v>8496364367</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="18">
+        <v>5452584566</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="18">
+        <v>54225585</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>